<commit_message>
Formata a coluna "Estimated Value" para o tipo currency e adiciona o símbolo da moeda. Adiciona uma tabela dinâmica Add e configura "Vendor Name" e "Production Month" como linhas , "Storage Zone" como coluna, e "Estimated Value" como valor usando soma. Adiciona um Gráfico para criar um gráfico de Colunas Stacked baseado na Tabela dinâmica. Atualiza o Título do Grafico para "Estimated Sales"
</commit_message>
<xml_diff>
--- a/Data/VegetablesProduction.xlsx
+++ b/Data/VegetablesProduction.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Adriano\Meus Arquivos\UiPath\Projetos\UipathAcademy\BasicProjects\CalculateEstimatedValue\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CE06EC-928B-441D-86AF-D1F0BD3A64F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474546A8-9B04-4122-BCD5-EA917D61A09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="2" r:id="rId1"/>
-    <sheet name="Tracker_Updated" sheetId="5" r:id="rId2"/>
+    <sheet name="Pivot Table" sheetId="6" r:id="rId2"/>
+    <sheet name="Tracker_Updated" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="44">
   <si>
     <t>Vegetables</t>
   </si>
@@ -146,16 +150,38 @@
   </si>
   <si>
     <t>Estimated Value</t>
+  </si>
+  <si>
+    <t>Rótulos de Linha</t>
+  </si>
+  <si>
+    <t>Total Geral</t>
+  </si>
+  <si>
+    <t>Rótulos de Coluna</t>
+  </si>
+  <si>
+    <t>Soma de Estimated Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$$]#,#00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,8 +207,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -198,6 +232,1529 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[VegetablesProduction.xlsx]Pivot Table!Pivot Table</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Estimated Sales</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:delete val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pivot Table'!$B$1:$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Pivot Table'!$A$3:$A$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>April</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>August</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>March</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>May</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>December</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>February</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>January</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>June</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>November</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>October</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>December</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>July</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>June</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>November</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>September</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>BFresh</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>EcoNGreen</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>VCrunch</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pivot Table'!$B$3:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="3">
+                  <c:v>3220.7999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7335.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A1C-448A-B54E-D07CCA5505AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pivot Table'!$C$1:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Pivot Table'!$A$3:$A$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>April</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>August</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>March</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>May</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>December</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>February</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>January</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>June</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>November</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>October</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>December</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>July</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>June</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>November</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>September</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>BFresh</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>EcoNGreen</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>VCrunch</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pivot Table'!$C$3:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="9">
+                  <c:v>1355.1999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3971.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7A1C-448A-B54E-D07CCA5505AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pivot Table'!$D$1:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Pivot Table'!$A$3:$A$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>April</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>August</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>March</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>May</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>December</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>February</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>January</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>June</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>November</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>October</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>December</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>July</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>June</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>November</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>September</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>BFresh</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>EcoNGreen</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>VCrunch</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pivot Table'!$D$3:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="14">
+                  <c:v>3187.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7A1C-448A-B54E-D07CCA5505AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pivot Table'!$E$1:$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>B1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Pivot Table'!$A$3:$A$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>April</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>August</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>March</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>May</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>December</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>February</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>January</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>June</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>November</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>October</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>December</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>July</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>June</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>November</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>September</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>BFresh</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>EcoNGreen</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>VCrunch</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pivot Table'!$E$3:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>3845.6000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6151.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9377.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-7A1C-448A-B54E-D07CCA5505AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pivot Table'!$F$1:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>B2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Pivot Table'!$A$3:$A$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>April</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>August</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>March</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>May</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>December</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>February</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>January</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>June</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>November</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>October</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>December</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>July</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>June</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>November</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>September</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>BFresh</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>EcoNGreen</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>VCrunch</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pivot Table'!$F$3:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="1">
+                  <c:v>3869.1000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3696</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-7A1C-448A-B54E-D07CCA5505AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pivot Table'!$G$1:$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Pivot Table'!$A$3:$A$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>April</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>August</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>March</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>May</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>December</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>February</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>January</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>June</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>November</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>October</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>December</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>July</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>June</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>November</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>September</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>BFresh</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>EcoNGreen</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>VCrunch</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pivot Table'!$G$3:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="4">
+                  <c:v>5126</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4292.3999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5478</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4316.8999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-7A1C-448A-B54E-D07CCA5505AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="744934447"/>
+        <c:axId val="720345055"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="744934447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="720345055"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="720345055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="744934447"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>71120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>386080</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{553D4CF7-3A1E-D266-452B-3041DC2A9ABF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Adriano Chanchinski" refreshedDate="45303.947438194446" createdVersion="1" refreshedVersion="8" recordCount="36" xr:uid="{BFD2D447-C8FA-4522-B1B3-A5B401D3D8F1}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:G37" sheet="Tracker_Updated"/>
+  </cacheSource>
+  <cacheFields count="7">
+    <cacheField name="Vegetables" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Production Month" numFmtId="0">
+      <sharedItems count="12">
+        <s v="September"/>
+        <s v="July"/>
+        <s v="May"/>
+        <s v="October"/>
+        <s v="August"/>
+        <s v="January"/>
+        <s v="April"/>
+        <s v="March"/>
+        <s v="November"/>
+        <s v="February"/>
+        <s v="December"/>
+        <s v="June"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Quantity" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="105" maxValue="996"/>
+    </cacheField>
+    <cacheField name="Storage Zone" numFmtId="0">
+      <sharedItems count="6">
+        <s v="A3"/>
+        <s v="A2"/>
+        <s v="A1"/>
+        <s v="B2"/>
+        <s v="B1"/>
+        <s v="C1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Vendor Name" numFmtId="0">
+      <sharedItems count="3">
+        <s v="VCrunch"/>
+        <s v="BFresh"/>
+        <s v="EcoNGreen"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Price per Kg" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.3" maxValue="6.6"/>
+    </cacheField>
+    <cacheField name="Estimated Value" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="231" maxValue="5478"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="36">
+  <r>
+    <s v="Pumpkins"/>
+    <x v="0"/>
+    <n v="782"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1.3"/>
+    <n v="1016.6"/>
+  </r>
+  <r>
+    <s v="Pumpkins"/>
+    <x v="0"/>
+    <n v="903"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1.3"/>
+    <n v="1173.9000000000001"/>
+  </r>
+  <r>
+    <s v="Pumpkins"/>
+    <x v="0"/>
+    <n v="767"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1.3"/>
+    <n v="997.1"/>
+  </r>
+  <r>
+    <s v="Onions"/>
+    <x v="1"/>
+    <n v="921"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1.6"/>
+    <n v="1473.6"/>
+  </r>
+  <r>
+    <s v="Onions"/>
+    <x v="1"/>
+    <n v="613"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1.6"/>
+    <n v="980.8"/>
+  </r>
+  <r>
+    <s v="Onions"/>
+    <x v="1"/>
+    <n v="948"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1.6"/>
+    <n v="1516.8"/>
+  </r>
+  <r>
+    <s v="Cucumbers"/>
+    <x v="2"/>
+    <n v="713"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2.2000000000000002"/>
+    <n v="1568.6"/>
+  </r>
+  <r>
+    <s v="Cucumbers"/>
+    <x v="2"/>
+    <n v="223"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2.2000000000000002"/>
+    <n v="490.6"/>
+  </r>
+  <r>
+    <s v="Cucumbers"/>
+    <x v="2"/>
+    <n v="528"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="2.2000000000000002"/>
+    <n v="1161.5999999999999"/>
+  </r>
+  <r>
+    <s v="Potatoes"/>
+    <x v="3"/>
+    <n v="324"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="2.2000000000000002"/>
+    <n v="712.8"/>
+  </r>
+  <r>
+    <s v="Potatoes"/>
+    <x v="3"/>
+    <n v="187"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="2.2000000000000002"/>
+    <n v="411.4"/>
+  </r>
+  <r>
+    <s v="Potatoes"/>
+    <x v="3"/>
+    <n v="105"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="2.2000000000000002"/>
+    <n v="231"/>
+  </r>
+  <r>
+    <s v="Squash"/>
+    <x v="4"/>
+    <n v="648"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="2.7"/>
+    <n v="1749.6"/>
+  </r>
+  <r>
+    <s v="Squash"/>
+    <x v="4"/>
+    <n v="246"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="2.7"/>
+    <n v="664.2"/>
+  </r>
+  <r>
+    <s v="Squash"/>
+    <x v="4"/>
+    <n v="539"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="2.7"/>
+    <n v="1455.3"/>
+  </r>
+  <r>
+    <s v="Carrots"/>
+    <x v="5"/>
+    <n v="573"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="3.3"/>
+    <n v="1890.9"/>
+  </r>
+  <r>
+    <s v="Carrots"/>
+    <x v="5"/>
+    <n v="782"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="3.3"/>
+    <n v="2580.6"/>
+  </r>
+  <r>
+    <s v="Carrots"/>
+    <x v="5"/>
+    <n v="868"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="3.3"/>
+    <n v="2864.4"/>
+  </r>
+  <r>
+    <s v="Lettuce"/>
+    <x v="6"/>
+    <n v="278"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="3.8"/>
+    <n v="1056.4000000000001"/>
+  </r>
+  <r>
+    <s v="Lettuce"/>
+    <x v="6"/>
+    <n v="455"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="3.8"/>
+    <n v="1729"/>
+  </r>
+  <r>
+    <s v="Lettuce"/>
+    <x v="6"/>
+    <n v="279"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="3.8"/>
+    <n v="1060.2"/>
+  </r>
+  <r>
+    <s v="Tomatoes"/>
+    <x v="7"/>
+    <n v="456"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="4.4000000000000004"/>
+    <n v="2006.4"/>
+  </r>
+  <r>
+    <s v="Tomatoes"/>
+    <x v="7"/>
+    <n v="798"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="4.4000000000000004"/>
+    <n v="3511.2"/>
+  </r>
+  <r>
+    <s v="Tomatoes"/>
+    <x v="7"/>
+    <n v="144"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="4.4000000000000004"/>
+    <n v="633.6"/>
+  </r>
+  <r>
+    <s v="Radishes"/>
+    <x v="8"/>
+    <n v="556"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="4.9000000000000004"/>
+    <n v="2724.4"/>
+  </r>
+  <r>
+    <s v="Radishes"/>
+    <x v="8"/>
+    <n v="325"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="4.9000000000000004"/>
+    <n v="1592.5"/>
+  </r>
+  <r>
+    <s v="Radishes"/>
+    <x v="8"/>
+    <n v="876"/>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="4.9000000000000004"/>
+    <n v="4292.3999999999996"/>
+  </r>
+  <r>
+    <s v="Broccoli"/>
+    <x v="9"/>
+    <n v="889"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="5.5"/>
+    <n v="4889.5"/>
+  </r>
+  <r>
+    <s v="Broccoli"/>
+    <x v="9"/>
+    <n v="129"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="5.5"/>
+    <n v="709.5"/>
+  </r>
+  <r>
+    <s v="Broccoli"/>
+    <x v="9"/>
+    <n v="687"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="5.5"/>
+    <n v="3778.5"/>
+  </r>
+  <r>
+    <s v="Beets"/>
+    <x v="10"/>
+    <n v="996"/>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="5.5"/>
+    <n v="5478"/>
+  </r>
+  <r>
+    <s v="Beets"/>
+    <x v="10"/>
+    <n v="679"/>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="5.5"/>
+    <n v="3734.5"/>
+  </r>
+  <r>
+    <s v="Beets"/>
+    <x v="10"/>
+    <n v="253"/>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="5.5"/>
+    <n v="1391.5"/>
+  </r>
+  <r>
+    <s v="Peppers"/>
+    <x v="11"/>
+    <n v="135"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="6.6"/>
+    <n v="891"/>
+  </r>
+  <r>
+    <s v="Peppers"/>
+    <x v="11"/>
+    <n v="425"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="6.6"/>
+    <n v="2805"/>
+  </r>
+  <r>
+    <s v="Peppers"/>
+    <x v="11"/>
+    <n v="625"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="6.6"/>
+    <n v="4125"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F6851A36-EA7B-49B9-BA15-0C06CE2C6FA4}" name="Pivot Table" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Dados" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1" chartFormat="1">
+  <location ref="A1:H21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" includeNewItemsInFilter="1">
+      <items count="13">
+        <item x="6"/>
+        <item x="4"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="11"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" includeNewItemsInFilter="1">
+      <items count="7">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" includeNewItemsInFilter="1">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="4"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="19">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Soma de Estimated Value" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="6">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1228,11 +2785,319 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38A42B8-A55C-40DE-BA5F-6F9794E727FF}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>3220.7999999999997</v>
+      </c>
+      <c r="E3">
+        <v>9996.8000000000011</v>
+      </c>
+      <c r="F3">
+        <v>3869.1000000000004</v>
+      </c>
+      <c r="H3">
+        <v>17086.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>3845.6000000000004</v>
+      </c>
+      <c r="H4">
+        <v>3845.6000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <v>3869.1000000000004</v>
+      </c>
+      <c r="H5">
+        <v>3869.1000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>6151.2000000000007</v>
+      </c>
+      <c r="H6">
+        <v>6151.2000000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>3220.7999999999997</v>
+      </c>
+      <c r="H7">
+        <v>3220.7999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>7335.9</v>
+      </c>
+      <c r="C8">
+        <v>1355.1999999999998</v>
+      </c>
+      <c r="E8">
+        <v>9377.5</v>
+      </c>
+      <c r="F8">
+        <v>3696</v>
+      </c>
+      <c r="G8">
+        <v>9418.4</v>
+      </c>
+      <c r="H8">
+        <v>31183.000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9">
+        <v>5126</v>
+      </c>
+      <c r="H9">
+        <v>5126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10">
+        <v>9377.5</v>
+      </c>
+      <c r="H10">
+        <v>9377.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>7335.9</v>
+      </c>
+      <c r="H11">
+        <v>7335.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12">
+        <v>3696</v>
+      </c>
+      <c r="H12">
+        <v>3696</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13">
+        <v>4292.3999999999996</v>
+      </c>
+      <c r="H13">
+        <v>4292.3999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>1355.1999999999998</v>
+      </c>
+      <c r="H14">
+        <v>1355.1999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>3971.2</v>
+      </c>
+      <c r="D15">
+        <v>3187.6</v>
+      </c>
+      <c r="F15">
+        <v>4125</v>
+      </c>
+      <c r="G15">
+        <v>9794.9</v>
+      </c>
+      <c r="H15">
+        <v>21078.699999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16">
+        <v>5478</v>
+      </c>
+      <c r="H16">
+        <v>5478</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>3971.2</v>
+      </c>
+      <c r="H17">
+        <v>3971.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18">
+        <v>4125</v>
+      </c>
+      <c r="H18">
+        <v>4125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19">
+        <v>4316.8999999999996</v>
+      </c>
+      <c r="H19">
+        <v>4316.8999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>3187.6</v>
+      </c>
+      <c r="H20">
+        <v>3187.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21">
+        <v>10556.699999999999</v>
+      </c>
+      <c r="C21">
+        <v>5326.4</v>
+      </c>
+      <c r="D21">
+        <v>3187.6</v>
+      </c>
+      <c r="E21">
+        <v>19374.300000000003</v>
+      </c>
+      <c r="F21">
+        <v>11690.1</v>
+      </c>
+      <c r="G21">
+        <v>19213.3</v>
+      </c>
+      <c r="H21">
+        <v>69348.399999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1240,10 +3105,10 @@
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1265,7 +3130,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1288,7 +3153,7 @@
       <c r="F2">
         <v>1.3</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>1016.6</v>
       </c>
     </row>
@@ -1311,7 +3176,7 @@
       <c r="F3">
         <v>1.3</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>1173.9000000000001</v>
       </c>
     </row>
@@ -1334,7 +3199,7 @@
       <c r="F4">
         <v>1.3</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>997.1</v>
       </c>
     </row>
@@ -1357,7 +3222,7 @@
       <c r="F5">
         <v>1.6</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>1473.6</v>
       </c>
     </row>
@@ -1380,7 +3245,7 @@
       <c r="F6">
         <v>1.6</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>980.8</v>
       </c>
     </row>
@@ -1403,7 +3268,7 @@
       <c r="F7">
         <v>1.6</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>1516.8</v>
       </c>
     </row>
@@ -1426,7 +3291,7 @@
       <c r="F8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>1568.6</v>
       </c>
     </row>
@@ -1449,7 +3314,7 @@
       <c r="F9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>490.6</v>
       </c>
     </row>
@@ -1472,7 +3337,7 @@
       <c r="F10">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>1161.5999999999999</v>
       </c>
     </row>
@@ -1495,7 +3360,7 @@
       <c r="F11">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>712.8</v>
       </c>
     </row>
@@ -1518,7 +3383,7 @@
       <c r="F12">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>411.4</v>
       </c>
     </row>
@@ -1541,7 +3406,7 @@
       <c r="F13">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>231</v>
       </c>
     </row>
@@ -1564,7 +3429,7 @@
       <c r="F14">
         <v>2.7</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>1749.6</v>
       </c>
     </row>
@@ -1587,7 +3452,7 @@
       <c r="F15">
         <v>2.7</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>664.2</v>
       </c>
     </row>
@@ -1610,7 +3475,7 @@
       <c r="F16">
         <v>2.7</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>1455.3</v>
       </c>
     </row>
@@ -1633,7 +3498,7 @@
       <c r="F17">
         <v>3.3</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>1890.9</v>
       </c>
     </row>
@@ -1656,7 +3521,7 @@
       <c r="F18">
         <v>3.3</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <v>2580.6</v>
       </c>
     </row>
@@ -1679,7 +3544,7 @@
       <c r="F19">
         <v>3.3</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <v>2864.4</v>
       </c>
     </row>
@@ -1702,7 +3567,7 @@
       <c r="F20">
         <v>3.8</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <v>1056.4000000000001</v>
       </c>
     </row>
@@ -1725,7 +3590,7 @@
       <c r="F21">
         <v>3.8</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <v>1729</v>
       </c>
     </row>
@@ -1748,7 +3613,7 @@
       <c r="F22">
         <v>3.8</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <v>1060.2</v>
       </c>
     </row>
@@ -1771,7 +3636,7 @@
       <c r="F23">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="1">
         <v>2006.4</v>
       </c>
     </row>
@@ -1794,7 +3659,7 @@
       <c r="F24">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="1">
         <v>3511.2</v>
       </c>
     </row>
@@ -1817,7 +3682,7 @@
       <c r="F25">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <v>633.6</v>
       </c>
     </row>
@@ -1840,7 +3705,7 @@
       <c r="F26">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
         <v>2724.4</v>
       </c>
     </row>
@@ -1863,7 +3728,7 @@
       <c r="F27">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="1">
         <v>1592.5</v>
       </c>
     </row>
@@ -1886,7 +3751,7 @@
       <c r="F28">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
         <v>4292.3999999999996</v>
       </c>
     </row>
@@ -1909,7 +3774,7 @@
       <c r="F29">
         <v>5.5</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="1">
         <v>4889.5</v>
       </c>
     </row>
@@ -1932,7 +3797,7 @@
       <c r="F30">
         <v>5.5</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
         <v>709.5</v>
       </c>
     </row>
@@ -1955,7 +3820,7 @@
       <c r="F31">
         <v>5.5</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="1">
         <v>3778.5</v>
       </c>
     </row>
@@ -1978,7 +3843,7 @@
       <c r="F32">
         <v>5.5</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="1">
         <v>5478</v>
       </c>
     </row>
@@ -2001,7 +3866,7 @@
       <c r="F33">
         <v>5.5</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
         <v>3734.5</v>
       </c>
     </row>
@@ -2024,7 +3889,7 @@
       <c r="F34">
         <v>5.5</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="1">
         <v>1391.5</v>
       </c>
     </row>
@@ -2047,7 +3912,7 @@
       <c r="F35">
         <v>6.6</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="1">
         <v>891</v>
       </c>
     </row>
@@ -2070,7 +3935,7 @@
       <c r="F36">
         <v>6.6</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="1">
         <v>2805</v>
       </c>
     </row>
@@ -2093,7 +3958,7 @@
       <c r="F37">
         <v>6.6</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="1">
         <v>4125</v>
       </c>
     </row>

</xml_diff>